<commit_message>
Completed validation on input.
</commit_message>
<xml_diff>
--- a/ex-autoprovision/autoprovision_site_list.xlsx
+++ b/ex-autoprovision/autoprovision_site_list.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hkeiken/git/mist-scripts-private/ex-autoprovision/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hkeiken/git/mist-scripts/ex-autoprovision/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C127B74-A819-414F-9EC3-EE1E69063C79}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10D7FAC4-3AC0-234D-B7C9-38DEEB3464FD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4300" yWindow="2760" windowWidth="27640" windowHeight="16940" xr2:uid="{E9134121-6A58-9F4D-9BFD-6DCEF951A100}"/>
   </bookViews>
@@ -36,34 +36,34 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
-    <t>Network</t>
-  </si>
-  <si>
-    <t>Site-id</t>
-  </si>
-  <si>
-    <t>Site-name</t>
-  </si>
-  <si>
-    <t>10.0.0.0/24</t>
-  </si>
-  <si>
-    <t>18bf02e3-8c11-4aef-b3f7-7a5284471c4f</t>
-  </si>
-  <si>
-    <t>Nordsetervegen 248</t>
-  </si>
-  <si>
-    <t>10.0.1.0/24</t>
-  </si>
-  <si>
-    <t>c8474fc3-8819-4cf0-b318-b7be37b21b7d</t>
-  </si>
-  <si>
-    <t>Test 2021-02</t>
-  </si>
-  <si>
     <t>id</t>
+  </si>
+  <si>
+    <t>network</t>
+  </si>
+  <si>
+    <t>site-id</t>
+  </si>
+  <si>
+    <t>site-name</t>
+  </si>
+  <si>
+    <t>10.10.10.0/24</t>
+  </si>
+  <si>
+    <t>10.10.11.0/24</t>
+  </si>
+  <si>
+    <t>abcf02e3-8c11-4aef-b3f7-7a5284471c4f</t>
+  </si>
+  <si>
+    <t>abc74fc3-8819-4cf0-b318-b7be37b21b7d</t>
+  </si>
+  <si>
+    <t>Site 1</t>
+  </si>
+  <si>
+    <t>Site 2</t>
   </si>
 </sst>
 </file>
@@ -418,7 +418,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -430,16 +430,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -447,13 +447,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -461,13 +461,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>